<commit_message>
undo retire experiment in senate district 16
</commit_message>
<xml_diff>
--- a/2022AssemblyMembers-geocoded.xlsx
+++ b/2022AssemblyMembers-geocoded.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epaulson/development/2024-maps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epaulson/development/2024-wisconsin-maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E26666-CC49-1149-8E85-FFEE2D2E15D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9551B412-96F0-8040-933E-76F547FBE75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="873">
   <si>
     <t>District</t>
   </si>
@@ -3011,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I86" sqref="I86"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5115,9 +5115,6 @@
       <c r="G48">
         <v>2016</v>
       </c>
-      <c r="H48" t="s">
-        <v>182</v>
-      </c>
       <c r="I48" t="s">
         <v>187</v>
       </c>
@@ -5161,9 +5158,6 @@
       </c>
       <c r="G49">
         <v>2020</v>
-      </c>
-      <c r="H49" t="s">
-        <v>182</v>
       </c>
       <c r="I49" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
Don't use Knodl's address since he left and was replaced, should have caught this earlier
</commit_message>
<xml_diff>
--- a/2022AssemblyMembers-geocoded.xlsx
+++ b/2022AssemblyMembers-geocoded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epaulson/development/2024-wisconsin-maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9551B412-96F0-8040-933E-76F547FBE75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99040134-0316-4A4F-ADCB-7428EBB6A022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,15 +304,9 @@
     <t>Paul Melotik</t>
   </si>
   <si>
-    <t>N101 W14475 RIDGEFIELD CT GERMANTOWN, 53022</t>
-  </si>
-  <si>
     <t>Grafton</t>
   </si>
   <si>
-    <t>43.2007373,-88.0890266</t>
-  </si>
-  <si>
     <t>Paul Tittl</t>
   </si>
   <si>
@@ -2639,6 +2633,12 @@
   </si>
   <si>
     <t>44.903275,-89.616184</t>
+  </si>
+  <si>
+    <t>1408 Pioneer Road Grafton, WI 53024</t>
+  </si>
+  <si>
+    <t>43.281988,-87.937524</t>
   </si>
 </sst>
 </file>
@@ -3011,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3057,22 +3057,22 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>382</v>
+      </c>
+      <c r="K1" t="s">
+        <v>383</v>
+      </c>
+      <c r="L1" t="s">
         <v>384</v>
       </c>
-      <c r="K1" t="s">
-        <v>385</v>
-      </c>
-      <c r="L1" t="s">
-        <v>386</v>
-      </c>
       <c r="M1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="N1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="O1" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -3101,19 +3101,19 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
+        <v>385</v>
+      </c>
+      <c r="K2" t="s">
+        <v>386</v>
+      </c>
+      <c r="L2" t="s">
         <v>387</v>
       </c>
-      <c r="K2" t="s">
-        <v>388</v>
-      </c>
-      <c r="L2" t="s">
-        <v>389</v>
-      </c>
       <c r="M2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="N2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -3145,19 +3145,19 @@
         <v>17</v>
       </c>
       <c r="J3" t="s">
+        <v>388</v>
+      </c>
+      <c r="K3" t="s">
+        <v>389</v>
+      </c>
+      <c r="L3" t="s">
         <v>390</v>
       </c>
-      <c r="K3" t="s">
-        <v>391</v>
-      </c>
-      <c r="L3" t="s">
-        <v>392</v>
-      </c>
       <c r="M3" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="N3" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -3189,19 +3189,19 @@
         <v>21</v>
       </c>
       <c r="J4" t="s">
+        <v>391</v>
+      </c>
+      <c r="K4" t="s">
+        <v>392</v>
+      </c>
+      <c r="L4" t="s">
         <v>393</v>
       </c>
-      <c r="K4" t="s">
-        <v>394</v>
-      </c>
-      <c r="L4" t="s">
-        <v>395</v>
-      </c>
       <c r="M4" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="N4" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="O4">
         <v>3</v>
@@ -3233,19 +3233,19 @@
         <v>25</v>
       </c>
       <c r="J5" t="s">
+        <v>394</v>
+      </c>
+      <c r="K5" t="s">
+        <v>395</v>
+      </c>
+      <c r="L5" t="s">
         <v>396</v>
       </c>
-      <c r="K5" t="s">
-        <v>397</v>
-      </c>
-      <c r="L5" t="s">
-        <v>398</v>
-      </c>
       <c r="M5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="N5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="O5">
         <v>4</v>
@@ -3274,19 +3274,19 @@
         <v>29</v>
       </c>
       <c r="J6" t="s">
+        <v>397</v>
+      </c>
+      <c r="K6" t="s">
+        <v>398</v>
+      </c>
+      <c r="L6" t="s">
         <v>399</v>
       </c>
-      <c r="K6" t="s">
-        <v>400</v>
-      </c>
-      <c r="L6" t="s">
-        <v>401</v>
-      </c>
       <c r="M6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="N6" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="O6">
         <v>5</v>
@@ -3318,19 +3318,19 @@
         <v>33</v>
       </c>
       <c r="J7" t="s">
+        <v>400</v>
+      </c>
+      <c r="K7" t="s">
+        <v>401</v>
+      </c>
+      <c r="L7" t="s">
         <v>402</v>
       </c>
-      <c r="K7" t="s">
-        <v>403</v>
-      </c>
-      <c r="L7" t="s">
-        <v>404</v>
-      </c>
       <c r="M7" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N7" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="O7">
         <v>6</v>
@@ -3362,19 +3362,19 @@
         <v>38</v>
       </c>
       <c r="J8" t="s">
+        <v>403</v>
+      </c>
+      <c r="K8" t="s">
+        <v>404</v>
+      </c>
+      <c r="L8" t="s">
         <v>405</v>
       </c>
-      <c r="K8" t="s">
-        <v>406</v>
-      </c>
-      <c r="L8" t="s">
-        <v>407</v>
-      </c>
       <c r="M8" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N8" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="O8">
         <v>7</v>
@@ -3403,19 +3403,19 @@
         <v>41</v>
       </c>
       <c r="J9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="K9" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M9" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="N9" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="O9">
         <v>8</v>
@@ -3447,19 +3447,19 @@
         <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="L10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M10" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="N10" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="O10">
         <v>9</v>
@@ -3491,19 +3491,19 @@
         <v>47</v>
       </c>
       <c r="J11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="K11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="L11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M11" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="N11" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="O11">
         <v>10</v>
@@ -3532,19 +3532,19 @@
         <v>50</v>
       </c>
       <c r="J12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M12" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N12" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="O12">
         <v>11</v>
@@ -3576,19 +3576,19 @@
         <v>53</v>
       </c>
       <c r="J13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="K13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="L13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M13" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="N13" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="O13">
         <v>12</v>
@@ -3620,19 +3620,19 @@
         <v>57</v>
       </c>
       <c r="J14" t="s">
+        <v>416</v>
+      </c>
+      <c r="K14" t="s">
+        <v>417</v>
+      </c>
+      <c r="L14" t="s">
         <v>418</v>
       </c>
-      <c r="K14" t="s">
-        <v>419</v>
-      </c>
-      <c r="L14" t="s">
-        <v>420</v>
-      </c>
       <c r="M14" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="N14" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="O14">
         <v>13</v>
@@ -3664,19 +3664,19 @@
         <v>61</v>
       </c>
       <c r="J15" t="s">
+        <v>419</v>
+      </c>
+      <c r="K15" t="s">
+        <v>420</v>
+      </c>
+      <c r="L15" t="s">
         <v>421</v>
       </c>
-      <c r="K15" t="s">
-        <v>422</v>
-      </c>
-      <c r="L15" t="s">
-        <v>423</v>
-      </c>
       <c r="M15" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="N15" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="O15">
         <v>13</v>
@@ -3708,19 +3708,19 @@
         <v>65</v>
       </c>
       <c r="J16" t="s">
+        <v>422</v>
+      </c>
+      <c r="K16" t="s">
+        <v>423</v>
+      </c>
+      <c r="L16" t="s">
         <v>424</v>
       </c>
-      <c r="K16" t="s">
-        <v>425</v>
-      </c>
-      <c r="L16" t="s">
-        <v>426</v>
-      </c>
       <c r="M16" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="N16" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="O16">
         <v>83</v>
@@ -3752,19 +3752,19 @@
         <v>68</v>
       </c>
       <c r="J17" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="K17" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="L17" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M17" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="N17" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="O17">
         <v>16</v>
@@ -3796,19 +3796,19 @@
         <v>71</v>
       </c>
       <c r="J18" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K18" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="L18" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M18" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="N18" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="O18">
         <v>17</v>
@@ -3840,19 +3840,19 @@
         <v>74</v>
       </c>
       <c r="J19" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K19" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="L19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M19" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="N19" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="O19">
         <v>18</v>
@@ -3884,19 +3884,19 @@
         <v>77</v>
       </c>
       <c r="J20" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K20" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L20" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M20" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="N20" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="O20">
         <v>19</v>
@@ -3928,19 +3928,19 @@
         <v>80</v>
       </c>
       <c r="J21" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="K21" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="L21" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M21" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N21" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O21">
         <v>20</v>
@@ -3972,19 +3972,19 @@
         <v>84</v>
       </c>
       <c r="J22" t="s">
+        <v>435</v>
+      </c>
+      <c r="K22" t="s">
+        <v>436</v>
+      </c>
+      <c r="L22" t="s">
         <v>437</v>
       </c>
-      <c r="K22" t="s">
-        <v>438</v>
-      </c>
-      <c r="L22" t="s">
-        <v>439</v>
-      </c>
       <c r="M22" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="N22" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="O22">
         <v>21</v>
@@ -4016,19 +4016,19 @@
         <v>88</v>
       </c>
       <c r="J23" t="s">
+        <v>438</v>
+      </c>
+      <c r="K23" t="s">
+        <v>439</v>
+      </c>
+      <c r="L23" t="s">
         <v>440</v>
       </c>
-      <c r="K23" t="s">
-        <v>441</v>
-      </c>
-      <c r="L23" t="s">
-        <v>442</v>
-      </c>
       <c r="M23" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="N23" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="O23">
         <v>24</v>
@@ -4060,19 +4060,19 @@
         <v>92</v>
       </c>
       <c r="J24" t="s">
+        <v>441</v>
+      </c>
+      <c r="K24" t="s">
+        <v>442</v>
+      </c>
+      <c r="L24" t="s">
         <v>443</v>
       </c>
-      <c r="K24" t="s">
-        <v>444</v>
-      </c>
-      <c r="L24" t="s">
-        <v>445</v>
-      </c>
       <c r="M24" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="N24" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="O24">
         <v>23</v>
@@ -4086,7 +4086,7 @@
         <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>871</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -4095,28 +4095,28 @@
         <v>66</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25">
         <v>2023</v>
       </c>
       <c r="I25" t="s">
-        <v>96</v>
+        <v>872</v>
       </c>
       <c r="J25" t="s">
+        <v>444</v>
+      </c>
+      <c r="K25" t="s">
+        <v>445</v>
+      </c>
+      <c r="L25" t="s">
         <v>446</v>
       </c>
-      <c r="K25" t="s">
-        <v>447</v>
-      </c>
-      <c r="L25" t="s">
-        <v>448</v>
-      </c>
       <c r="M25" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="N25" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="O25">
         <v>24</v>
@@ -4127,10 +4127,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -4139,28 +4139,28 @@
         <v>61</v>
       </c>
       <c r="F26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G26">
         <v>2012</v>
       </c>
       <c r="I26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J26" t="s">
+        <v>447</v>
+      </c>
+      <c r="K26" t="s">
+        <v>448</v>
+      </c>
+      <c r="L26" t="s">
         <v>449</v>
       </c>
-      <c r="K26" t="s">
-        <v>450</v>
-      </c>
-      <c r="L26" t="s">
-        <v>451</v>
-      </c>
       <c r="M26" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="N26" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="O26">
         <v>25</v>
@@ -4171,10 +4171,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -4183,28 +4183,28 @@
         <v>64</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G27">
         <v>2014</v>
       </c>
       <c r="I27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J27" t="s">
+        <v>450</v>
+      </c>
+      <c r="K27" t="s">
+        <v>451</v>
+      </c>
+      <c r="L27" t="s">
         <v>452</v>
       </c>
-      <c r="K27" t="s">
-        <v>453</v>
-      </c>
-      <c r="L27" t="s">
-        <v>454</v>
-      </c>
       <c r="M27" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="N27" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="O27">
         <v>27</v>
@@ -4215,10 +4215,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -4227,28 +4227,28 @@
         <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G28">
         <v>2022</v>
       </c>
       <c r="I28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J28" t="s">
+        <v>453</v>
+      </c>
+      <c r="K28" t="s">
+        <v>454</v>
+      </c>
+      <c r="L28" t="s">
         <v>455</v>
       </c>
-      <c r="K28" t="s">
-        <v>456</v>
-      </c>
-      <c r="L28" t="s">
-        <v>457</v>
-      </c>
       <c r="M28" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="N28" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="O28">
         <v>25</v>
@@ -4259,10 +4259,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -4271,28 +4271,28 @@
         <v>70</v>
       </c>
       <c r="F29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G29">
         <v>2018</v>
       </c>
       <c r="I29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J29" t="s">
+        <v>456</v>
+      </c>
+      <c r="K29" t="s">
+        <v>457</v>
+      </c>
+      <c r="L29" t="s">
         <v>458</v>
       </c>
-      <c r="K29" t="s">
-        <v>459</v>
-      </c>
-      <c r="L29" t="s">
-        <v>460</v>
-      </c>
       <c r="M29" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N29" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="O29">
         <v>75</v>
@@ -4303,10 +4303,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -4315,28 +4315,28 @@
         <v>46</v>
       </c>
       <c r="F30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G30">
         <v>2020</v>
       </c>
       <c r="I30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J30" t="s">
+        <v>459</v>
+      </c>
+      <c r="K30" t="s">
+        <v>460</v>
+      </c>
+      <c r="L30" t="s">
         <v>461</v>
       </c>
-      <c r="K30" t="s">
-        <v>462</v>
-      </c>
-      <c r="L30" t="s">
-        <v>463</v>
-      </c>
       <c r="M30" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="N30" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="O30">
         <v>92</v>
@@ -4347,10 +4347,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -4359,28 +4359,28 @@
         <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G31">
         <v>2016</v>
       </c>
       <c r="I31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J31" t="s">
+        <v>462</v>
+      </c>
+      <c r="K31" t="s">
+        <v>463</v>
+      </c>
+      <c r="L31" t="s">
         <v>464</v>
       </c>
-      <c r="K31" t="s">
-        <v>465</v>
-      </c>
-      <c r="L31" t="s">
-        <v>466</v>
-      </c>
       <c r="M31" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="N31" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="O31">
         <v>30</v>
@@ -4391,10 +4391,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -4403,28 +4403,28 @@
         <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G32">
         <v>2022</v>
       </c>
       <c r="I32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J32" t="s">
+        <v>465</v>
+      </c>
+      <c r="K32" t="s">
+        <v>466</v>
+      </c>
+      <c r="L32" t="s">
         <v>467</v>
       </c>
-      <c r="K32" t="s">
-        <v>468</v>
-      </c>
-      <c r="L32" t="s">
-        <v>469</v>
-      </c>
       <c r="M32" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="N32" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="O32">
         <v>31</v>
@@ -4435,10 +4435,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -4447,28 +4447,28 @@
         <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G33">
         <v>2010</v>
       </c>
       <c r="I33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J33" t="s">
+        <v>468</v>
+      </c>
+      <c r="K33" t="s">
+        <v>469</v>
+      </c>
+      <c r="L33" t="s">
         <v>470</v>
       </c>
-      <c r="K33" t="s">
-        <v>471</v>
-      </c>
-      <c r="L33" t="s">
-        <v>472</v>
-      </c>
       <c r="M33" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="N33" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="O33">
         <v>32</v>
@@ -4479,10 +4479,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -4491,28 +4491,28 @@
         <v>69</v>
       </c>
       <c r="F34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G34">
         <v>2022</v>
       </c>
       <c r="I34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J34" t="s">
+        <v>471</v>
+      </c>
+      <c r="K34" t="s">
+        <v>472</v>
+      </c>
+      <c r="L34" t="s">
         <v>473</v>
       </c>
-      <c r="K34" t="s">
-        <v>474</v>
-      </c>
-      <c r="L34" t="s">
-        <v>475</v>
-      </c>
       <c r="M34" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="N34" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="O34">
         <v>97</v>
@@ -4523,10 +4523,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -4535,28 +4535,28 @@
         <v>59</v>
       </c>
       <c r="F35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G35">
         <v>2012</v>
       </c>
       <c r="I35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J35" t="s">
+        <v>474</v>
+      </c>
+      <c r="K35" t="s">
+        <v>475</v>
+      </c>
+      <c r="L35" t="s">
         <v>476</v>
       </c>
-      <c r="K35" t="s">
-        <v>477</v>
-      </c>
-      <c r="L35" t="s">
-        <v>478</v>
-      </c>
       <c r="M35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="N35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="O35">
         <v>34</v>
@@ -4567,10 +4567,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -4579,28 +4579,28 @@
         <v>23</v>
       </c>
       <c r="F36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G36">
         <v>2020</v>
       </c>
       <c r="I36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J36" t="s">
+        <v>477</v>
+      </c>
+      <c r="K36" t="s">
+        <v>478</v>
+      </c>
+      <c r="L36" t="s">
         <v>479</v>
       </c>
-      <c r="K36" t="s">
-        <v>480</v>
-      </c>
-      <c r="L36" t="s">
-        <v>481</v>
-      </c>
       <c r="M36" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="N36" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="O36">
         <v>35</v>
@@ -4611,10 +4611,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -4623,28 +4623,28 @@
         <v>68</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G37">
         <v>2004</v>
       </c>
       <c r="I37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J37" t="s">
+        <v>480</v>
+      </c>
+      <c r="K37" t="s">
+        <v>481</v>
+      </c>
+      <c r="L37" t="s">
         <v>482</v>
       </c>
-      <c r="K37" t="s">
-        <v>483</v>
-      </c>
-      <c r="L37" t="s">
-        <v>484</v>
-      </c>
       <c r="M37" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="N37" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="O37">
         <v>36</v>
@@ -4655,10 +4655,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -4667,28 +4667,28 @@
         <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G38">
         <v>2021</v>
       </c>
       <c r="I38" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="J38" t="s">
+        <v>483</v>
+      </c>
+      <c r="K38" t="s">
+        <v>484</v>
+      </c>
+      <c r="L38" t="s">
         <v>485</v>
       </c>
-      <c r="K38" t="s">
-        <v>486</v>
-      </c>
-      <c r="L38" t="s">
-        <v>487</v>
-      </c>
       <c r="M38" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="N38" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="O38">
         <v>42</v>
@@ -4699,10 +4699,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -4711,28 +4711,28 @@
         <v>58</v>
       </c>
       <c r="F39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G39">
         <v>2018</v>
       </c>
       <c r="I39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J39" t="s">
+        <v>486</v>
+      </c>
+      <c r="K39" t="s">
+        <v>487</v>
+      </c>
+      <c r="L39" t="s">
         <v>488</v>
       </c>
-      <c r="K39" t="s">
-        <v>489</v>
-      </c>
-      <c r="L39" t="s">
-        <v>490</v>
-      </c>
       <c r="M39" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="N39" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="O39">
         <v>99</v>
@@ -4743,10 +4743,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -4755,28 +4755,28 @@
         <v>46</v>
       </c>
       <c r="F40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G40">
         <v>2012</v>
       </c>
       <c r="I40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J40" t="s">
+        <v>489</v>
+      </c>
+      <c r="K40" t="s">
+        <v>490</v>
+      </c>
+      <c r="L40" t="s">
         <v>491</v>
       </c>
-      <c r="K40" t="s">
-        <v>492</v>
-      </c>
-      <c r="L40" t="s">
-        <v>493</v>
-      </c>
       <c r="M40" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="N40" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="O40">
         <v>37</v>
@@ -4787,10 +4787,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -4799,28 +4799,28 @@
         <v>58</v>
       </c>
       <c r="F41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G41">
         <v>2006</v>
       </c>
       <c r="I41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J41" t="s">
+        <v>492</v>
+      </c>
+      <c r="K41" t="s">
+        <v>493</v>
+      </c>
+      <c r="L41" t="s">
         <v>494</v>
       </c>
-      <c r="K41" t="s">
-        <v>495</v>
-      </c>
-      <c r="L41" t="s">
-        <v>496</v>
-      </c>
       <c r="M41" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="N41" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="O41">
         <v>57</v>
@@ -4831,10 +4831,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -4843,28 +4843,28 @@
         <v>30</v>
       </c>
       <c r="F42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G42">
         <v>2020</v>
       </c>
       <c r="I42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J42" t="s">
+        <v>495</v>
+      </c>
+      <c r="K42" t="s">
+        <v>496</v>
+      </c>
+      <c r="L42" t="s">
         <v>497</v>
       </c>
-      <c r="K42" t="s">
-        <v>498</v>
-      </c>
-      <c r="L42" t="s">
-        <v>499</v>
-      </c>
       <c r="M42" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="N42" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="O42">
         <v>39</v>
@@ -4875,10 +4875,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -4887,28 +4887,28 @@
         <v>67</v>
       </c>
       <c r="F43" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G43">
         <v>2018</v>
       </c>
       <c r="I43" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J43" t="s">
+        <v>498</v>
+      </c>
+      <c r="K43" t="s">
+        <v>499</v>
+      </c>
+      <c r="L43" t="s">
         <v>500</v>
       </c>
-      <c r="K43" t="s">
-        <v>501</v>
-      </c>
-      <c r="L43" t="s">
-        <v>502</v>
-      </c>
       <c r="M43" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N43" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="O43">
         <v>42</v>
@@ -4919,10 +4919,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D44" t="s">
         <v>36</v>
@@ -4931,28 +4931,28 @@
         <v>41</v>
       </c>
       <c r="F44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G44">
         <v>2022</v>
       </c>
       <c r="I44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J44" t="s">
+        <v>501</v>
+      </c>
+      <c r="K44" t="s">
+        <v>502</v>
+      </c>
+      <c r="L44" t="s">
         <v>503</v>
       </c>
-      <c r="K44" t="s">
-        <v>504</v>
-      </c>
-      <c r="L44" t="s">
-        <v>505</v>
-      </c>
       <c r="M44" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="N44" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="O44">
         <v>50</v>
@@ -4963,10 +4963,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C45" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D45" t="s">
         <v>36</v>
@@ -4975,28 +4975,28 @@
         <v>62</v>
       </c>
       <c r="F45" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G45">
         <v>2020</v>
       </c>
       <c r="I45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J45" t="s">
+        <v>504</v>
+      </c>
+      <c r="K45" t="s">
+        <v>505</v>
+      </c>
+      <c r="L45" t="s">
         <v>506</v>
       </c>
-      <c r="K45" t="s">
-        <v>507</v>
-      </c>
-      <c r="L45" t="s">
-        <v>508</v>
-      </c>
       <c r="M45" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="N45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="O45">
         <v>44</v>
@@ -5007,10 +5007,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D46" t="s">
         <v>36</v>
@@ -5019,28 +5019,28 @@
         <v>29</v>
       </c>
       <c r="F46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G46">
         <v>2022</v>
       </c>
       <c r="I46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J46" t="s">
+        <v>507</v>
+      </c>
+      <c r="K46" t="s">
+        <v>508</v>
+      </c>
+      <c r="L46" t="s">
         <v>509</v>
       </c>
-      <c r="K46" t="s">
-        <v>510</v>
-      </c>
-      <c r="L46" t="s">
-        <v>511</v>
-      </c>
       <c r="M46" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="N46" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="O46">
         <v>45</v>
@@ -5051,10 +5051,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D47" t="s">
         <v>36</v>
@@ -5063,31 +5063,31 @@
         <v>46</v>
       </c>
       <c r="F47" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G47">
         <v>2022</v>
       </c>
       <c r="H47" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I47" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J47" t="s">
+        <v>510</v>
+      </c>
+      <c r="K47" t="s">
+        <v>511</v>
+      </c>
+      <c r="L47" t="s">
         <v>512</v>
       </c>
-      <c r="K47" t="s">
-        <v>513</v>
-      </c>
-      <c r="L47" t="s">
-        <v>514</v>
-      </c>
       <c r="M47" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="N47" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="O47">
         <v>46</v>
@@ -5098,10 +5098,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C48" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D48" t="s">
         <v>36</v>
@@ -5110,28 +5110,28 @@
         <v>36</v>
       </c>
       <c r="F48" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G48">
         <v>2016</v>
       </c>
       <c r="I48" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J48" t="s">
+        <v>513</v>
+      </c>
+      <c r="K48" t="s">
+        <v>514</v>
+      </c>
+      <c r="L48" t="s">
         <v>515</v>
       </c>
-      <c r="K48" t="s">
-        <v>516</v>
-      </c>
-      <c r="L48" t="s">
-        <v>517</v>
-      </c>
       <c r="M48" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="N48" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="O48">
         <v>47</v>
@@ -5142,10 +5142,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C49" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D49" t="s">
         <v>36</v>
@@ -5154,28 +5154,28 @@
         <v>52</v>
       </c>
       <c r="F49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G49">
         <v>2020</v>
       </c>
       <c r="I49" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J49" t="s">
+        <v>516</v>
+      </c>
+      <c r="K49" t="s">
+        <v>517</v>
+      </c>
+      <c r="L49" t="s">
         <v>518</v>
       </c>
-      <c r="K49" t="s">
-        <v>519</v>
-      </c>
-      <c r="L49" t="s">
-        <v>520</v>
-      </c>
       <c r="M49" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="N49" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="O49">
         <v>48</v>
@@ -5186,10 +5186,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C50" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
@@ -5198,28 +5198,28 @@
         <v>37</v>
       </c>
       <c r="F50" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G50">
         <v>2010</v>
       </c>
       <c r="I50" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J50" t="s">
+        <v>519</v>
+      </c>
+      <c r="K50" t="s">
+        <v>520</v>
+      </c>
+      <c r="L50" t="s">
         <v>521</v>
       </c>
-      <c r="K50" t="s">
-        <v>522</v>
-      </c>
-      <c r="L50" t="s">
-        <v>523</v>
-      </c>
       <c r="M50" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N50" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="O50">
         <v>49</v>
@@ -5230,10 +5230,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C51" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
@@ -5242,28 +5242,28 @@
         <v>56</v>
       </c>
       <c r="F51" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G51">
         <v>2018</v>
       </c>
       <c r="I51" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J51" t="s">
+        <v>522</v>
+      </c>
+      <c r="K51" t="s">
+        <v>523</v>
+      </c>
+      <c r="L51" t="s">
         <v>524</v>
       </c>
-      <c r="K51" t="s">
-        <v>525</v>
-      </c>
-      <c r="L51" t="s">
-        <v>526</v>
-      </c>
       <c r="M51" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="N51" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="O51">
         <v>41</v>
@@ -5274,10 +5274,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
@@ -5286,28 +5286,28 @@
         <v>57</v>
       </c>
       <c r="F52" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G52">
         <v>2014</v>
       </c>
       <c r="I52" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J52" t="s">
+        <v>525</v>
+      </c>
+      <c r="K52" t="s">
+        <v>526</v>
+      </c>
+      <c r="L52" t="s">
         <v>527</v>
       </c>
-      <c r="K52" t="s">
-        <v>528</v>
-      </c>
-      <c r="L52" t="s">
-        <v>529</v>
-      </c>
       <c r="M52" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="N52" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="O52">
         <v>51</v>
@@ -5318,10 +5318,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C53" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
@@ -5330,28 +5330,28 @@
         <v>69</v>
       </c>
       <c r="F53" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G53">
         <v>2022</v>
       </c>
       <c r="I53" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J53" t="s">
+        <v>528</v>
+      </c>
+      <c r="K53" t="s">
+        <v>529</v>
+      </c>
+      <c r="L53" t="s">
         <v>530</v>
       </c>
-      <c r="K53" t="s">
-        <v>531</v>
-      </c>
-      <c r="L53" t="s">
-        <v>532</v>
-      </c>
       <c r="M53" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="N53" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="O53">
         <v>60</v>
@@ -5362,10 +5362,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C54" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -5374,28 +5374,28 @@
         <v>61</v>
       </c>
       <c r="F54" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G54">
         <v>2012</v>
       </c>
       <c r="I54" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J54" t="s">
+        <v>531</v>
+      </c>
+      <c r="K54" t="s">
+        <v>532</v>
+      </c>
+      <c r="L54" t="s">
         <v>533</v>
       </c>
-      <c r="K54" t="s">
-        <v>534</v>
-      </c>
-      <c r="L54" t="s">
-        <v>535</v>
-      </c>
       <c r="M54" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="N54" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="O54">
         <v>55</v>
@@ -5406,10 +5406,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D55" t="s">
         <v>36</v>
@@ -5418,28 +5418,28 @@
         <v>55</v>
       </c>
       <c r="F55" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G55">
         <v>2022</v>
       </c>
       <c r="I55" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J55" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="K55" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="L55" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="M55" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="N55" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="O55">
         <v>54</v>
@@ -5450,10 +5450,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C56" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -5462,28 +5462,28 @@
         <v>28</v>
       </c>
       <c r="F56" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G56">
         <v>2022</v>
       </c>
       <c r="I56" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J56" t="s">
+        <v>536</v>
+      </c>
+      <c r="K56" t="s">
+        <v>537</v>
+      </c>
+      <c r="L56" t="s">
         <v>538</v>
       </c>
-      <c r="K56" t="s">
-        <v>539</v>
-      </c>
-      <c r="L56" t="s">
-        <v>540</v>
-      </c>
       <c r="M56" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="N56" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="O56">
         <v>55</v>
@@ -5494,10 +5494,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C57" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
@@ -5506,28 +5506,28 @@
         <v>68</v>
       </c>
       <c r="F57" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G57">
         <v>2012</v>
       </c>
       <c r="I57" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J57" t="s">
+        <v>539</v>
+      </c>
+      <c r="K57" t="s">
+        <v>540</v>
+      </c>
+      <c r="L57" t="s">
         <v>541</v>
       </c>
-      <c r="K57" t="s">
-        <v>542</v>
-      </c>
-      <c r="L57" t="s">
-        <v>543</v>
-      </c>
       <c r="M57" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="N57" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="O57">
         <v>56</v>
@@ -5538,10 +5538,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C58" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D58" t="s">
         <v>36</v>
@@ -5550,28 +5550,28 @@
         <v>53</v>
       </c>
       <c r="F58" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G58">
         <v>2020</v>
       </c>
       <c r="I58" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J58" t="s">
+        <v>542</v>
+      </c>
+      <c r="K58" t="s">
+        <v>543</v>
+      </c>
+      <c r="L58" t="s">
         <v>544</v>
       </c>
-      <c r="K58" t="s">
-        <v>545</v>
-      </c>
-      <c r="L58" t="s">
-        <v>546</v>
-      </c>
       <c r="M58" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="N58" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="O58">
         <v>52</v>
@@ -5582,10 +5582,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C59" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -5594,28 +5594,28 @@
         <v>57</v>
       </c>
       <c r="F59" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G59">
         <v>2018</v>
       </c>
       <c r="I59" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J59" t="s">
+        <v>545</v>
+      </c>
+      <c r="K59" t="s">
+        <v>546</v>
+      </c>
+      <c r="L59" t="s">
         <v>547</v>
       </c>
-      <c r="K59" t="s">
-        <v>548</v>
-      </c>
-      <c r="L59" t="s">
-        <v>549</v>
-      </c>
       <c r="M59" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="N59" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="O59">
         <v>58</v>
@@ -5626,10 +5626,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C60" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -5638,28 +5638,28 @@
         <v>29</v>
       </c>
       <c r="F60" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G60">
         <v>2022</v>
       </c>
       <c r="I60" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J60" t="s">
+        <v>548</v>
+      </c>
+      <c r="K60" t="s">
+        <v>549</v>
+      </c>
+      <c r="L60" t="s">
         <v>550</v>
       </c>
-      <c r="K60" t="s">
-        <v>551</v>
-      </c>
-      <c r="L60" t="s">
-        <v>552</v>
-      </c>
       <c r="M60" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="N60" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="O60">
         <v>3</v>
@@ -5670,10 +5670,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C61" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -5682,28 +5682,28 @@
         <v>57</v>
       </c>
       <c r="F61" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G61">
         <v>2014</v>
       </c>
       <c r="I61" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J61" t="s">
+        <v>551</v>
+      </c>
+      <c r="K61" t="s">
+        <v>552</v>
+      </c>
+      <c r="L61" t="s">
         <v>553</v>
       </c>
-      <c r="K61" t="s">
-        <v>554</v>
-      </c>
-      <c r="L61" t="s">
-        <v>555</v>
-      </c>
       <c r="M61" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="N61" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="O61">
         <v>59</v>
@@ -5714,10 +5714,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -5726,28 +5726,28 @@
         <v>47</v>
       </c>
       <c r="F62" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G62">
         <v>2022</v>
       </c>
       <c r="I62" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J62" t="s">
+        <v>554</v>
+      </c>
+      <c r="K62" t="s">
+        <v>555</v>
+      </c>
+      <c r="L62" t="s">
         <v>556</v>
       </c>
-      <c r="K62" t="s">
-        <v>557</v>
-      </c>
-      <c r="L62" t="s">
-        <v>558</v>
-      </c>
       <c r="M62" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="N62" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="O62">
         <v>32</v>
@@ -5758,10 +5758,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C63" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
@@ -5770,28 +5770,28 @@
         <v>65</v>
       </c>
       <c r="F63" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G63">
         <v>2018</v>
       </c>
       <c r="I63" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J63" t="s">
+        <v>557</v>
+      </c>
+      <c r="K63" t="s">
+        <v>558</v>
+      </c>
+      <c r="L63" t="s">
         <v>559</v>
       </c>
-      <c r="K63" t="s">
-        <v>560</v>
-      </c>
-      <c r="L63" t="s">
-        <v>561</v>
-      </c>
       <c r="M63" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="N63" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="O63">
         <v>62</v>
@@ -5802,10 +5802,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C64" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -5814,28 +5814,28 @@
         <v>54</v>
       </c>
       <c r="F64" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G64">
         <v>2004</v>
       </c>
       <c r="I64" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J64" t="s">
+        <v>560</v>
+      </c>
+      <c r="K64" t="s">
+        <v>561</v>
+      </c>
+      <c r="L64" t="s">
         <v>562</v>
       </c>
-      <c r="K64" t="s">
-        <v>563</v>
-      </c>
-      <c r="L64" t="s">
-        <v>564</v>
-      </c>
       <c r="M64" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="N64" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="O64">
         <v>33</v>
@@ -5846,10 +5846,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C65" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D65" t="s">
         <v>36</v>
@@ -5858,28 +5858,28 @@
         <v>36</v>
       </c>
       <c r="F65" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G65">
         <v>2019</v>
       </c>
       <c r="I65" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J65" t="s">
+        <v>563</v>
+      </c>
+      <c r="K65" t="s">
+        <v>564</v>
+      </c>
+      <c r="L65" t="s">
         <v>565</v>
       </c>
-      <c r="K65" t="s">
-        <v>566</v>
-      </c>
-      <c r="L65" t="s">
-        <v>567</v>
-      </c>
       <c r="M65" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="N65" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="O65">
         <v>64</v>
@@ -5890,10 +5890,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C66" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D66" t="s">
         <v>36</v>
@@ -5902,28 +5902,28 @@
         <v>70</v>
       </c>
       <c r="F66" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G66">
         <v>2012</v>
       </c>
       <c r="I66" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J66" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="K66" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="L66" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="M66" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="N66" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="O66">
         <v>65</v>
@@ -5934,10 +5934,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C67" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D67" t="s">
         <v>36</v>
@@ -5946,28 +5946,28 @@
         <v>31</v>
       </c>
       <c r="F67" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G67">
         <v>2018</v>
       </c>
       <c r="I67" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J67" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="K67" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="L67" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="M67" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="N67" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="O67">
         <v>62</v>
@@ -5978,10 +5978,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C68" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -5990,28 +5990,28 @@
         <v>42</v>
       </c>
       <c r="F68" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G68">
         <v>2016</v>
       </c>
       <c r="I68" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J68" t="s">
+        <v>570</v>
+      </c>
+      <c r="K68" t="s">
+        <v>571</v>
+      </c>
+      <c r="L68" t="s">
         <v>572</v>
       </c>
-      <c r="K68" t="s">
-        <v>573</v>
-      </c>
-      <c r="L68" t="s">
-        <v>574</v>
-      </c>
       <c r="M68" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="N68" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="O68">
         <v>68</v>
@@ -6022,10 +6022,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C69" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -6034,28 +6034,28 @@
         <v>50</v>
       </c>
       <c r="F69" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G69">
         <v>2022</v>
       </c>
       <c r="I69" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J69" t="s">
+        <v>573</v>
+      </c>
+      <c r="K69" t="s">
+        <v>574</v>
+      </c>
+      <c r="L69" t="s">
         <v>575</v>
       </c>
-      <c r="K69" t="s">
-        <v>576</v>
-      </c>
-      <c r="L69" t="s">
-        <v>577</v>
-      </c>
       <c r="M69" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="N69" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="O69">
         <v>91</v>
@@ -6066,10 +6066,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C70" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
@@ -6078,28 +6078,28 @@
         <v>72</v>
       </c>
       <c r="F70" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G70">
         <v>2020</v>
       </c>
       <c r="I70" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J70" t="s">
+        <v>576</v>
+      </c>
+      <c r="K70" t="s">
+        <v>577</v>
+      </c>
+      <c r="L70" t="s">
         <v>578</v>
       </c>
-      <c r="K70" t="s">
-        <v>579</v>
-      </c>
-      <c r="L70" t="s">
-        <v>580</v>
-      </c>
       <c r="M70" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="N70" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="O70">
         <v>86</v>
@@ -6110,10 +6110,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C71" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -6122,28 +6122,28 @@
         <v>64</v>
       </c>
       <c r="F71" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G71">
         <v>2014</v>
       </c>
       <c r="I71" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J71" t="s">
+        <v>579</v>
+      </c>
+      <c r="K71" t="s">
+        <v>580</v>
+      </c>
+      <c r="L71" t="s">
         <v>581</v>
       </c>
-      <c r="K71" t="s">
-        <v>582</v>
-      </c>
-      <c r="L71" t="s">
-        <v>583</v>
-      </c>
       <c r="M71" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="N71" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="O71">
         <v>70</v>
@@ -6154,10 +6154,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C72" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D72" t="s">
         <v>36</v>
@@ -6166,31 +6166,31 @@
         <v>35</v>
       </c>
       <c r="F72" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G72">
         <v>2012</v>
       </c>
       <c r="H72" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I72" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J72" t="s">
+        <v>582</v>
+      </c>
+      <c r="K72" t="s">
+        <v>583</v>
+      </c>
+      <c r="L72" t="s">
         <v>584</v>
       </c>
-      <c r="K72" t="s">
-        <v>585</v>
-      </c>
-      <c r="L72" t="s">
-        <v>586</v>
-      </c>
       <c r="M72" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="N72" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="O72">
         <v>71</v>
@@ -6201,10 +6201,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C73" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
@@ -6213,28 +6213,28 @@
         <v>47</v>
       </c>
       <c r="F73" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G73">
         <v>2010</v>
       </c>
       <c r="I73" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J73" t="s">
+        <v>585</v>
+      </c>
+      <c r="K73" t="s">
+        <v>586</v>
+      </c>
+      <c r="L73" t="s">
         <v>587</v>
       </c>
-      <c r="K73" t="s">
-        <v>588</v>
-      </c>
-      <c r="L73" t="s">
-        <v>589</v>
-      </c>
       <c r="M73" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="N73" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="O73">
         <v>72</v>
@@ -6245,10 +6245,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C74" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
@@ -6257,28 +6257,28 @@
         <v>38</v>
       </c>
       <c r="F74" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G74">
         <v>2022</v>
       </c>
       <c r="I74" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J74" t="s">
+        <v>588</v>
+      </c>
+      <c r="K74" t="s">
+        <v>589</v>
+      </c>
+      <c r="L74" t="s">
         <v>590</v>
       </c>
-      <c r="K74" t="s">
-        <v>591</v>
-      </c>
-      <c r="L74" t="s">
-        <v>592</v>
-      </c>
       <c r="M74" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="N74" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="O74">
         <v>73</v>
@@ -6289,10 +6289,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C75" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D75" t="s">
         <v>11</v>
@@ -6301,28 +6301,28 @@
         <v>32</v>
       </c>
       <c r="F75" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G75">
         <v>2022</v>
       </c>
       <c r="I75" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J75" t="s">
+        <v>591</v>
+      </c>
+      <c r="K75" t="s">
+        <v>592</v>
+      </c>
+      <c r="L75" t="s">
         <v>593</v>
       </c>
-      <c r="K75" t="s">
-        <v>594</v>
-      </c>
-      <c r="L75" t="s">
-        <v>595</v>
-      </c>
       <c r="M75" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="N75" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="O75">
         <v>74</v>
@@ -6333,10 +6333,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C76" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D76" t="s">
         <v>11</v>
@@ -6345,28 +6345,28 @@
         <v>61</v>
       </c>
       <c r="F76" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G76">
         <v>2020</v>
       </c>
       <c r="I76" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J76" t="s">
+        <v>594</v>
+      </c>
+      <c r="K76" t="s">
+        <v>595</v>
+      </c>
+      <c r="L76" t="s">
         <v>596</v>
       </c>
-      <c r="K76" t="s">
-        <v>597</v>
-      </c>
-      <c r="L76" t="s">
-        <v>598</v>
-      </c>
       <c r="M76" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="N76" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="O76">
         <v>67</v>
@@ -6377,10 +6377,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C77" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D77" t="s">
         <v>36</v>
@@ -6389,28 +6389,28 @@
         <v>34</v>
       </c>
       <c r="F77" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G77">
         <v>2020</v>
       </c>
       <c r="I77" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J77" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="K77" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L77" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="M77" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="N77" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="O77">
         <v>76</v>
@@ -6421,10 +6421,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C78" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D78" t="s">
         <v>36</v>
@@ -6433,28 +6433,28 @@
         <v>51</v>
       </c>
       <c r="F78" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G78">
         <v>2018</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="J78" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="K78" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L78" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="M78" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="N78" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="O78">
         <v>78</v>
@@ -6465,10 +6465,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C79" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D79" t="s">
         <v>36</v>
@@ -6477,28 +6477,28 @@
         <v>51</v>
       </c>
       <c r="F79" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G79">
         <v>2014</v>
       </c>
       <c r="I79" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J79" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K79" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L79" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="M79" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="N79" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="O79">
         <v>79</v>
@@ -6509,10 +6509,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C80" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D80" t="s">
         <v>36</v>
@@ -6521,28 +6521,28 @@
         <v>31</v>
       </c>
       <c r="F80" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G80">
         <v>2022</v>
       </c>
       <c r="I80" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J80" t="s">
+        <v>603</v>
+      </c>
+      <c r="K80" t="s">
+        <v>604</v>
+      </c>
+      <c r="L80" t="s">
         <v>605</v>
       </c>
-      <c r="K80" t="s">
-        <v>606</v>
-      </c>
-      <c r="L80" t="s">
-        <v>607</v>
-      </c>
       <c r="M80" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="N80" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="O80">
         <v>80</v>
@@ -6553,10 +6553,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C81" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D81" t="s">
         <v>36</v>
@@ -6565,28 +6565,28 @@
         <v>37</v>
       </c>
       <c r="F81" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G81">
         <v>2022</v>
       </c>
       <c r="I81" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J81" t="s">
+        <v>606</v>
+      </c>
+      <c r="K81" t="s">
+        <v>607</v>
+      </c>
+      <c r="L81" t="s">
         <v>608</v>
       </c>
-      <c r="K81" t="s">
-        <v>609</v>
-      </c>
-      <c r="L81" t="s">
-        <v>610</v>
-      </c>
       <c r="M81" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="N81" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="O81">
         <v>80</v>
@@ -6597,10 +6597,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C82" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D82" t="s">
         <v>36</v>
@@ -6609,31 +6609,31 @@
         <v>70</v>
       </c>
       <c r="F82" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G82">
         <v>2014</v>
       </c>
       <c r="H82" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I82" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J82" t="s">
+        <v>609</v>
+      </c>
+      <c r="K82" t="s">
+        <v>610</v>
+      </c>
+      <c r="L82" t="s">
         <v>611</v>
       </c>
-      <c r="K82" t="s">
-        <v>612</v>
-      </c>
-      <c r="L82" t="s">
-        <v>613</v>
-      </c>
       <c r="M82" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="N82" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="O82">
         <v>40</v>
@@ -6644,10 +6644,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C83" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D83" t="s">
         <v>11</v>
@@ -6656,28 +6656,28 @@
         <v>57</v>
       </c>
       <c r="F83" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G83">
         <v>2016</v>
       </c>
       <c r="I83" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J83" t="s">
+        <v>612</v>
+      </c>
+      <c r="K83" t="s">
+        <v>613</v>
+      </c>
+      <c r="L83" t="s">
         <v>614</v>
       </c>
-      <c r="K83" t="s">
-        <v>615</v>
-      </c>
-      <c r="L83" t="s">
-        <v>616</v>
-      </c>
       <c r="M83" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="N83" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="O83">
         <v>84</v>
@@ -6688,10 +6688,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C84" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
@@ -6700,28 +6700,28 @@
         <v>32</v>
       </c>
       <c r="F84" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G84">
         <v>2022</v>
       </c>
       <c r="I84" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J84" t="s">
+        <v>615</v>
+      </c>
+      <c r="K84" t="s">
+        <v>616</v>
+      </c>
+      <c r="L84" t="s">
         <v>617</v>
       </c>
-      <c r="K84" t="s">
-        <v>618</v>
-      </c>
-      <c r="L84" t="s">
-        <v>619</v>
-      </c>
       <c r="M84" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="N84" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="O84">
         <v>84</v>
@@ -6732,10 +6732,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C85" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D85" t="s">
         <v>11</v>
@@ -6744,28 +6744,28 @@
         <v>67</v>
       </c>
       <c r="F85" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G85">
         <v>2022</v>
       </c>
       <c r="I85" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J85" t="s">
+        <v>618</v>
+      </c>
+      <c r="K85" t="s">
+        <v>619</v>
+      </c>
+      <c r="L85" t="s">
         <v>620</v>
       </c>
-      <c r="K85" t="s">
-        <v>621</v>
-      </c>
-      <c r="L85" t="s">
-        <v>622</v>
-      </c>
       <c r="M85" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="N85" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="O85">
         <v>7</v>
@@ -6776,10 +6776,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C86" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D86" t="s">
         <v>11</v>
@@ -6788,28 +6788,28 @@
         <v>66</v>
       </c>
       <c r="F86" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G86">
         <v>2016</v>
       </c>
       <c r="I86" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="J86" t="s">
+        <v>621</v>
+      </c>
+      <c r="K86" t="s">
+        <v>622</v>
+      </c>
+      <c r="L86" t="s">
         <v>623</v>
       </c>
-      <c r="K86" t="s">
-        <v>624</v>
-      </c>
-      <c r="L86" t="s">
-        <v>625</v>
-      </c>
       <c r="M86" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="N86" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="O86">
         <v>87</v>
@@ -6820,10 +6820,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C87" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D87" t="s">
         <v>11</v>
@@ -6832,28 +6832,28 @@
         <v>61</v>
       </c>
       <c r="F87" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G87">
         <v>2012</v>
       </c>
       <c r="I87" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="J87" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K87" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="L87" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="M87" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="N87" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="O87">
         <v>86</v>
@@ -6864,10 +6864,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C88" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D88" t="s">
         <v>11</v>
@@ -6876,28 +6876,28 @@
         <v>77</v>
       </c>
       <c r="F88" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G88">
         <v>2014</v>
       </c>
       <c r="I88" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J88" t="s">
+        <v>626</v>
+      </c>
+      <c r="K88" t="s">
+        <v>627</v>
+      </c>
+      <c r="L88" t="s">
         <v>628</v>
       </c>
-      <c r="K88" t="s">
-        <v>629</v>
-      </c>
-      <c r="L88" t="s">
-        <v>630</v>
-      </c>
       <c r="M88" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="N88" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="O88">
         <v>68</v>
@@ -6908,10 +6908,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C89" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
@@ -6920,28 +6920,28 @@
         <v>64</v>
       </c>
       <c r="F89" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G89">
         <v>2014</v>
       </c>
       <c r="I89" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J89" t="s">
+        <v>629</v>
+      </c>
+      <c r="K89" t="s">
+        <v>630</v>
+      </c>
+      <c r="L89" t="s">
         <v>631</v>
       </c>
-      <c r="K89" t="s">
-        <v>632</v>
-      </c>
-      <c r="L89" t="s">
-        <v>633</v>
-      </c>
       <c r="M89" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="N89" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="O89">
         <v>2</v>
@@ -6952,10 +6952,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C90" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D90" t="s">
         <v>11</v>
@@ -6964,28 +6964,28 @@
         <v>39</v>
       </c>
       <c r="F90" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G90">
         <v>2021</v>
       </c>
       <c r="I90" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="J90" t="s">
+        <v>632</v>
+      </c>
+      <c r="K90" t="s">
+        <v>633</v>
+      </c>
+      <c r="L90" t="s">
         <v>634</v>
       </c>
-      <c r="K90" t="s">
-        <v>635</v>
-      </c>
-      <c r="L90" t="s">
-        <v>636</v>
-      </c>
       <c r="M90" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="N90" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="O90">
         <v>4</v>
@@ -6996,10 +6996,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C91" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D91" t="s">
         <v>36</v>
@@ -7014,22 +7014,22 @@
         <v>2020</v>
       </c>
       <c r="I91" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="J91" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K91" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="L91" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M91" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="N91" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="O91">
         <v>90</v>
@@ -7040,10 +7040,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C92" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D92" t="s">
         <v>36</v>
@@ -7052,28 +7052,28 @@
         <v>49</v>
       </c>
       <c r="F92" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G92">
         <v>2018</v>
       </c>
       <c r="I92" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J92" t="s">
+        <v>637</v>
+      </c>
+      <c r="K92" t="s">
+        <v>638</v>
+      </c>
+      <c r="L92" t="s">
         <v>639</v>
       </c>
-      <c r="K92" t="s">
-        <v>640</v>
-      </c>
-      <c r="L92" t="s">
-        <v>641</v>
-      </c>
       <c r="M92" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="N92" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="O92">
         <v>91</v>
@@ -7084,10 +7084,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C93" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
@@ -7096,28 +7096,28 @@
         <v>55</v>
       </c>
       <c r="F93" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G93">
         <v>2016</v>
       </c>
       <c r="I93" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="J93" t="s">
+        <v>640</v>
+      </c>
+      <c r="K93" t="s">
+        <v>641</v>
+      </c>
+      <c r="L93" t="s">
         <v>642</v>
       </c>
-      <c r="K93" t="s">
-        <v>643</v>
-      </c>
-      <c r="L93" t="s">
-        <v>644</v>
-      </c>
       <c r="M93" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="N93" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O93">
         <v>29</v>
@@ -7128,10 +7128,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C94" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D94" t="s">
         <v>11</v>
@@ -7140,28 +7140,28 @@
         <v>67</v>
       </c>
       <c r="F94" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G94">
         <v>2010</v>
       </c>
       <c r="I94" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J94" t="s">
+        <v>643</v>
+      </c>
+      <c r="K94" t="s">
+        <v>644</v>
+      </c>
+      <c r="L94" t="s">
         <v>645</v>
       </c>
-      <c r="K94" t="s">
-        <v>646</v>
-      </c>
-      <c r="L94" t="s">
-        <v>647</v>
-      </c>
       <c r="M94" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="N94" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="O94">
         <v>93</v>
@@ -7172,10 +7172,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C95" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D95" t="s">
         <v>36</v>
@@ -7184,28 +7184,28 @@
         <v>64</v>
       </c>
       <c r="F95" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G95">
         <v>2011</v>
       </c>
       <c r="I95" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J95" t="s">
+        <v>646</v>
+      </c>
+      <c r="K95" t="s">
+        <v>647</v>
+      </c>
+      <c r="L95" t="s">
         <v>648</v>
       </c>
-      <c r="K95" t="s">
-        <v>649</v>
-      </c>
-      <c r="L95" t="s">
-        <v>650</v>
-      </c>
       <c r="M95" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="N95" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="O95">
         <v>94</v>
@@ -7216,10 +7216,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C96" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D96" t="s">
         <v>36</v>
@@ -7228,28 +7228,28 @@
         <v>58</v>
       </c>
       <c r="F96" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G96">
         <v>2011</v>
       </c>
       <c r="I96" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J96" t="s">
+        <v>649</v>
+      </c>
+      <c r="K96" t="s">
+        <v>650</v>
+      </c>
+      <c r="L96" t="s">
         <v>651</v>
       </c>
-      <c r="K96" t="s">
-        <v>652</v>
-      </c>
-      <c r="L96" t="s">
-        <v>653</v>
-      </c>
       <c r="M96" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="N96" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="O96">
         <v>95</v>
@@ -7260,10 +7260,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C97" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D97" t="s">
         <v>11</v>
@@ -7272,28 +7272,28 @@
         <v>57</v>
       </c>
       <c r="F97" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G97">
         <v>2018</v>
       </c>
       <c r="I97" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J97" t="s">
+        <v>652</v>
+      </c>
+      <c r="K97" t="s">
+        <v>653</v>
+      </c>
+      <c r="L97" t="s">
         <v>654</v>
       </c>
-      <c r="K97" t="s">
-        <v>655</v>
-      </c>
-      <c r="L97" t="s">
-        <v>656</v>
-      </c>
       <c r="M97" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="N97" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="O97">
         <v>96</v>
@@ -7304,10 +7304,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C98" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D98" t="s">
         <v>11</v>
@@ -7316,28 +7316,28 @@
         <v>57</v>
       </c>
       <c r="F98" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G98">
         <v>2014</v>
       </c>
       <c r="I98" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J98" t="s">
+        <v>655</v>
+      </c>
+      <c r="K98" t="s">
+        <v>656</v>
+      </c>
+      <c r="L98" t="s">
         <v>657</v>
       </c>
-      <c r="K98" t="s">
-        <v>658</v>
-      </c>
-      <c r="L98" t="s">
-        <v>659</v>
-      </c>
       <c r="M98" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="N98" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="O98">
         <v>82</v>
@@ -7348,10 +7348,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C99" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D99" t="s">
         <v>11</v>
@@ -7360,28 +7360,28 @@
         <v>38</v>
       </c>
       <c r="F99" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G99">
         <v>2013</v>
       </c>
       <c r="I99" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J99" t="s">
+        <v>658</v>
+      </c>
+      <c r="K99" t="s">
+        <v>659</v>
+      </c>
+      <c r="L99" t="s">
         <v>660</v>
       </c>
-      <c r="K99" t="s">
-        <v>661</v>
-      </c>
-      <c r="L99" t="s">
-        <v>662</v>
-      </c>
       <c r="M99" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="N99" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="O99">
         <v>15</v>
@@ -7392,10 +7392,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C100" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D100" t="s">
         <v>11</v>
@@ -7404,28 +7404,28 @@
         <v>64</v>
       </c>
       <c r="F100" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G100">
         <v>2015</v>
       </c>
       <c r="I100" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J100" t="s">
+        <v>661</v>
+      </c>
+      <c r="K100" t="s">
+        <v>662</v>
+      </c>
+      <c r="L100" t="s">
         <v>663</v>
       </c>
-      <c r="K100" t="s">
-        <v>664</v>
-      </c>
-      <c r="L100" t="s">
-        <v>665</v>
-      </c>
       <c r="M100" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="N100" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="O100">
         <v>97</v>

</xml_diff>

<commit_message>
finish updates from the knodl change
</commit_message>
<xml_diff>
--- a/2022AssemblyMembers-geocoded.xlsx
+++ b/2022AssemblyMembers-geocoded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/epaulson/development/2024-wisconsin-maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99040134-0316-4A4F-ADCB-7428EBB6A022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBA4297-2D9F-C242-A719-1FEC6769C86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3011,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4119,7 +4119,7 @@
         <v>715</v>
       </c>
       <c r="O25">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>